<commit_message>
Getting somewhere with Analysis, all Reformat I think is good.
Up next: Important to test the actual rows but population is nearing complete
</commit_message>
<xml_diff>
--- a/v300Track_this.xlsx
+++ b/v300Track_this.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/provider-type-status-breakdown/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C89F44-3F9D-7A4D-8F52-5EC6FCBB2B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1965B279-84C1-BA43-817F-E9FCB7821DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{E854799E-52F4-964A-8115-FB73305101DE}"/>
+    <workbookView xWindow="960" yWindow="4480" windowWidth="24160" windowHeight="17120" activeTab="2" xr2:uid="{E854799E-52F4-964A-8115-FB73305101DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="198">
   <si>
     <t>CITY</t>
   </si>
@@ -145,12 +145,6 @@
     <t>OUTPATIENT_HEALTH_TREATMENT_CENTER_REPORT (TRC)</t>
   </si>
   <si>
-    <t>Seller Leads</t>
-  </si>
-  <si>
-    <t>Survey Leads</t>
-  </si>
-  <si>
     <t>PROVIDER</t>
   </si>
   <si>
@@ -181,15 +175,9 @@
     <t>Total Blanks</t>
   </si>
   <si>
-    <t>Total SOLO PROVIDER TYPE PROVIDER</t>
-  </si>
-  <si>
     <t>Total PROVIDER</t>
   </si>
   <si>
-    <t>Total PROVIDER GROUP</t>
-  </si>
-  <si>
     <t>COUNTY</t>
   </si>
   <si>
@@ -629,13 +617,28 @@
   </si>
   <si>
     <t>Reinstated PROVIDER TYPE, Existing ADDRESS</t>
+  </si>
+  <si>
+    <t>Total Seller Lead</t>
+  </si>
+  <si>
+    <t>Total Seller/Survey Lead</t>
+  </si>
+  <si>
+    <t>Total Survey Lead</t>
+  </si>
+  <si>
+    <t>Total PROVIDER_GROUP</t>
+  </si>
+  <si>
+    <t>Total SOLO_PROVIDER_TYPE_PROVIDER_[Y,#]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -692,24 +695,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF268BD2"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -841,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -868,31 +857,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1229,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831D24BA-37DE-294C-9250-5A4F79049A63}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,35 +1233,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>197</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1291,56 +1273,56 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1352,116 +1334,117 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="6"/>
+        <v>194</v>
+      </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>193</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
+      <c r="A33" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
     </row>
@@ -1520,8 +1503,14 @@
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1546,7 +1535,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1567,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1637,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC809DA1-636D-084F-8ADA-9C195DB81B8B}">
-  <dimension ref="A1:FB36"/>
+  <dimension ref="A1:FC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="EN6" sqref="EN6"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1657,15 +1646,15 @@
     <col min="138" max="155" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:158" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:159" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -1677,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1689,379 +1678,379 @@
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="R1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="Y1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="Z1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="AA1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="AB1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AE1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AF1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AG1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AH1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AL1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AM1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AN1" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AP1" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AQ1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AR1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="AP1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AZ1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="BA1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="BB1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="AY1" s="14" t="s">
+      <c r="BC1" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BD1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="BA1" s="14" t="s">
+      <c r="BE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BB1" s="14" t="s">
+      <c r="BF1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BC1" s="14" t="s">
+      <c r="BG1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BD1" s="14" t="s">
+      <c r="BH1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CR1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CS1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CT1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CU1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="CR1" s="10" t="s">
+      <c r="CV1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="CS1" s="10" t="s">
+      <c r="CW1" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="CT1" s="10" t="s">
+      <c r="CX1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="CU1" s="10" t="s">
+      <c r="CY1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="CV1" s="11" t="s">
+      <c r="CZ1" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="CW1" s="11" t="s">
+      <c r="DA1" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="CX1" s="11" t="s">
+      <c r="DB1" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="CY1" s="11" t="s">
+      <c r="DC1" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="CZ1" s="10" t="s">
+      <c r="DD1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="DA1" s="10" t="s">
+      <c r="DE1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="DB1" s="10" t="s">
+      <c r="DF1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="DC1" s="10" t="s">
+      <c r="DG1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="DD1" s="10" t="s">
+      <c r="DH1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="DE1" s="10" t="s">
+      <c r="DI1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="DF1" s="10" t="s">
+      <c r="DJ1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="DG1" s="10" t="s">
+      <c r="DK1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="DH1" s="10" t="s">
+      <c r="DL1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="DI1" s="10" t="s">
+      <c r="DM1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="DJ1" s="10" t="s">
+      <c r="DN1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="DK1" s="10" t="s">
+      <c r="DO1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="DL1" s="10" t="s">
+      <c r="DP1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="DM1" s="10" t="s">
+      <c r="DQ1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="DN1" s="10" t="s">
+      <c r="DR1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="DO1" s="10" t="s">
+      <c r="DS1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="DP1" s="10" t="s">
+      <c r="DT1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="DQ1" s="10" t="s">
+      <c r="DU1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="DR1" s="10" t="s">
+      <c r="DV1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="DS1" s="10" t="s">
+      <c r="DW1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="DT1" s="10" t="s">
+      <c r="DX1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="DU1" s="10" t="s">
+      <c r="DY1" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="DV1" s="10" t="s">
+      <c r="DZ1" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="DW1" s="10" t="s">
+      <c r="EA1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="DX1" s="10" t="s">
+      <c r="EB1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="DY1" s="10" t="s">
+      <c r="EC1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="DZ1" s="10" t="s">
+      <c r="ED1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="EA1" s="10" t="s">
+      <c r="EE1" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="EB1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="EC1" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="ED1" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="EE1" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="EF1" s="12" t="s">
         <v>21</v>
@@ -2069,62 +2058,62 @@
       <c r="EG1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="EH1" s="26" t="s">
+      <c r="EH1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="EI1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="EJ1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="EK1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="EL1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="EI1" s="26" t="s">
+      <c r="EM1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="EJ1" s="26" t="s">
+      <c r="EN1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="EK1" s="26" t="s">
+      <c r="EO1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="EL1" s="26" t="s">
+      <c r="EP1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="EM1" s="26" t="s">
+      <c r="EQ1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="EN1" s="26" t="s">
+      <c r="ER1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="EO1" s="26" t="s">
+      <c r="ES1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="EP1" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="EQ1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="ER1" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="ES1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="ET1" s="26" t="s">
+      <c r="ET1" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="EU1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="EV1" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="EW1" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="EX1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="EU1" s="26" t="s">
+      <c r="EY1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="EV1" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="EW1" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="EX1" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="EY1" s="26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:158" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:159" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2136,7 +2125,6 @@
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
-      <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
@@ -2261,9 +2249,9 @@
       <c r="ED2"/>
       <c r="EE2"/>
       <c r="EF2"/>
-      <c r="EG2" s="18"/>
-    </row>
-    <row r="3" spans="1:158" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="EG2" s="16"/>
+    </row>
+    <row r="3" spans="1:159" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -2400,19 +2388,19 @@
       <c r="ED3"/>
       <c r="EE3"/>
       <c r="EF3"/>
-      <c r="EG3" s="18"/>
-      <c r="EJ3" s="20"/>
-      <c r="EK3" s="20"/>
-      <c r="EM3" s="20"/>
-      <c r="EN3" s="20"/>
-      <c r="EO3" s="23"/>
-      <c r="EP3" s="23"/>
-      <c r="ES3" s="20"/>
-      <c r="EW3" s="20"/>
-      <c r="EX3" s="20"/>
-      <c r="EY3" s="24"/>
-    </row>
-    <row r="4" spans="1:158" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="EG3" s="16"/>
+      <c r="EJ3" s="18"/>
+      <c r="EK3" s="18"/>
+      <c r="EM3" s="18"/>
+      <c r="EN3" s="18"/>
+      <c r="EO3" s="20"/>
+      <c r="EP3" s="20"/>
+      <c r="ES3" s="18"/>
+      <c r="EW3" s="18"/>
+      <c r="EX3" s="18"/>
+      <c r="EY3" s="21"/>
+    </row>
+    <row r="4" spans="1:159" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -2428,11 +2416,11 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
       <c r="U4"/>
       <c r="V4"/>
       <c r="W4"/>
@@ -2549,74 +2537,69 @@
       <c r="ED4"/>
       <c r="EE4"/>
       <c r="EF4"/>
-      <c r="EG4" s="18"/>
-      <c r="EH4" s="21"/>
-      <c r="EI4" s="21"/>
-      <c r="EJ4" s="21"/>
-      <c r="EK4" s="21"/>
-      <c r="EL4" s="21"/>
-      <c r="EM4" s="21"/>
-      <c r="EN4" s="21"/>
-      <c r="EO4" s="21"/>
-      <c r="EP4" s="21"/>
-      <c r="EQ4" s="21"/>
-      <c r="ER4" s="21"/>
-      <c r="ES4" s="21"/>
-      <c r="ET4" s="21"/>
-      <c r="EU4" s="21"/>
-      <c r="EV4" s="21"/>
-      <c r="EW4" s="21"/>
-      <c r="EX4" s="21"/>
-      <c r="EY4" s="21"/>
-      <c r="EZ4" s="21"/>
-      <c r="FA4" s="21"/>
-      <c r="FB4" s="21"/>
-    </row>
-    <row r="5" spans="1:158" x14ac:dyDescent="0.2">
+      <c r="EG4"/>
+      <c r="EH4"/>
+      <c r="EI4"/>
+      <c r="EJ4"/>
+      <c r="EK4"/>
+      <c r="EL4"/>
+      <c r="EM4"/>
+      <c r="EN4"/>
+      <c r="EO4"/>
+      <c r="EP4"/>
+      <c r="EQ4"/>
+      <c r="ER4"/>
+      <c r="ES4"/>
+      <c r="ET4"/>
+      <c r="EU4"/>
+      <c r="EV4"/>
+      <c r="EW4"/>
+      <c r="EX4"/>
+      <c r="EY4"/>
+      <c r="EZ4"/>
+      <c r="FA4"/>
+      <c r="FB4"/>
+      <c r="FC4"/>
+    </row>
+    <row r="5" spans="1:159" x14ac:dyDescent="0.2">
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="EH5" s="17"/>
-      <c r="EI5" s="17"/>
-      <c r="EJ5" s="17"/>
-      <c r="EK5" s="17"/>
-      <c r="EL5" s="17"/>
-      <c r="EM5" s="17"/>
-    </row>
-    <row r="6" spans="1:158" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:159" x14ac:dyDescent="0.2">
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
     </row>
-    <row r="7" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:159" x14ac:dyDescent="0.2">
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:159" x14ac:dyDescent="0.2">
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="12" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:159" x14ac:dyDescent="0.2">
       <c r="CY12" s="3"/>
     </row>
-    <row r="13" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:159" x14ac:dyDescent="0.2">
       <c r="CY13" s="3"/>
     </row>
-    <row r="14" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:159" x14ac:dyDescent="0.2">
       <c r="CY14" s="3"/>
     </row>
     <row r="36" spans="144:144" x14ac:dyDescent="0.2">
-      <c r="EN36" s="25"/>
+      <c r="EN36" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>